<commit_message>
Fixing months that were changed to numbers in fixed dataset
</commit_message>
<xml_diff>
--- a/data/marburg/fixed/marburg_fixing.xlsx
+++ b/data/marburg/fixed/marburg_fixing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gc4018\Documents\code\priority-pathogens\data\marburg\fixing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/kem22_ic_ac_uk/Documents/Projects/Priority Pathogens/priority-pathogens/data/marburg/fixed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F2C0215-8C5E-43C2-A789-CC83B05F0BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{1F2C0215-8C5E-43C2-A789-CC83B05F0BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F95D902-850E-43D0-93C2-A3E2508AB91E}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{ABF3DFDB-71ED-41C9-97C7-A2F6B992A437}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ABF3DFDB-71ED-41C9-97C7-A2F6B992A437}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="569">
   <si>
     <t>fixed</t>
   </si>
@@ -1764,13 +1764,25 @@
     <t/>
   </si>
   <si>
-    <t>March</t>
-  </si>
-  <si>
     <t>2013</t>
   </si>
   <si>
-    <t>June</t>
+    <t>Jan 01</t>
+  </si>
+  <si>
+    <t>Nov 11</t>
+  </si>
+  <si>
+    <t>Mar 03</t>
+  </si>
+  <si>
+    <t>Sep 09</t>
+  </si>
+  <si>
+    <t>Jul 07</t>
+  </si>
+  <si>
+    <t>Jun 06</t>
   </si>
 </sst>
 </file>
@@ -1930,7 +1942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1959,24 +1971,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2311,19 +2310,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B4796A1-9A3D-4303-832B-A1FBABA24A2A}">
-  <dimension ref="A1:BE21"/>
+  <dimension ref="A1:BE42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="AH17" workbookViewId="0">
+      <selection activeCell="AX24" sqref="AX24:AX42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2490,7 +2489,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -2657,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A3" t="b">
         <v>1</v>
       </c>
@@ -2796,8 +2795,8 @@
       <c r="AT3" t="s">
         <v>58</v>
       </c>
-      <c r="AU3" s="2">
-        <v>40848</v>
+      <c r="AU3" s="25" t="s">
+        <v>564</v>
       </c>
       <c r="AV3">
         <v>1981</v>
@@ -2805,8 +2804,8 @@
       <c r="AW3" t="s">
         <v>58</v>
       </c>
-      <c r="AX3" s="2">
-        <v>36892</v>
+      <c r="AX3" s="25" t="s">
+        <v>563</v>
       </c>
       <c r="AY3">
         <v>1982</v>
@@ -2824,7 +2823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A4" t="b">
         <v>1</v>
       </c>
@@ -2963,7 +2962,7 @@
       <c r="AT4" t="s">
         <v>58</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AU4" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AV4" t="s">
@@ -2972,7 +2971,7 @@
       <c r="AW4" t="s">
         <v>58</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="AX4" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AY4" t="s">
@@ -2991,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -3130,7 +3129,7 @@
       <c r="AT5" t="s">
         <v>58</v>
       </c>
-      <c r="AU5" t="s">
+      <c r="AU5" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AV5">
@@ -3139,7 +3138,7 @@
       <c r="AW5" t="s">
         <v>58</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="AX5" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AY5">
@@ -3158,7 +3157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -3297,7 +3296,7 @@
       <c r="AT6" t="s">
         <v>58</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AU6" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AV6">
@@ -3306,7 +3305,7 @@
       <c r="AW6" t="s">
         <v>58</v>
       </c>
-      <c r="AX6" t="s">
+      <c r="AX6" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AY6">
@@ -3325,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A7" t="b">
         <v>1</v>
       </c>
@@ -3464,7 +3463,7 @@
       <c r="AT7" t="s">
         <v>58</v>
       </c>
-      <c r="AU7" t="s">
+      <c r="AU7" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AV7">
@@ -3473,7 +3472,7 @@
       <c r="AW7" t="s">
         <v>58</v>
       </c>
-      <c r="AX7" t="s">
+      <c r="AX7" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AY7">
@@ -3492,7 +3491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -3631,7 +3630,7 @@
       <c r="AT8" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AU8" s="20" t="s">
+      <c r="AU8" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AV8" s="20" t="s">
@@ -3640,7 +3639,7 @@
       <c r="AW8" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AX8" s="20" t="s">
+      <c r="AX8" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AY8" s="20" t="s">
@@ -3661,7 +3660,7 @@
       <c r="BD8" s="20"/>
       <c r="BE8" s="20"/>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A9" t="b">
         <v>1</v>
       </c>
@@ -3800,7 +3799,7 @@
       <c r="AT9" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AU9" s="20" t="s">
+      <c r="AU9" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AV9" s="20" t="s">
@@ -3809,7 +3808,7 @@
       <c r="AW9" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AX9" s="20" t="s">
+      <c r="AX9" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AY9" s="20" t="s">
@@ -3830,7 +3829,7 @@
       <c r="BD9" s="20"/>
       <c r="BE9" s="20"/>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A10" t="b">
         <v>1</v>
       </c>
@@ -3969,7 +3968,7 @@
       <c r="AT10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AU10" s="20" t="s">
+      <c r="AU10" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AV10" s="20" t="s">
@@ -3978,7 +3977,7 @@
       <c r="AW10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AX10" s="20" t="s">
+      <c r="AX10" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AY10" s="20" t="s">
@@ -3999,7 +3998,7 @@
       <c r="BD10" s="20"/>
       <c r="BE10" s="20"/>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A11" t="b">
         <v>1</v>
       </c>
@@ -4138,7 +4137,7 @@
       <c r="AT11" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AU11" s="20" t="s">
+      <c r="AU11" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AV11" s="20" t="s">
@@ -4147,7 +4146,7 @@
       <c r="AW11" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AX11" s="20" t="s">
+      <c r="AX11" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AY11" s="20" t="s">
@@ -4168,7 +4167,7 @@
       <c r="BD11" s="20"/>
       <c r="BE11" s="20"/>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -4307,7 +4306,7 @@
       <c r="AT12" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AU12" s="20" t="s">
+      <c r="AU12" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AV12" s="20" t="s">
@@ -4316,7 +4315,7 @@
       <c r="AW12" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AX12" s="20" t="s">
+      <c r="AX12" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AY12" s="20" t="s">
@@ -4337,7 +4336,7 @@
       <c r="BD12" s="20"/>
       <c r="BE12" s="20"/>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A13" t="b">
         <v>1</v>
       </c>
@@ -4476,7 +4475,7 @@
       <c r="AT13" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AU13" s="20" t="s">
+      <c r="AU13" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AV13" s="20" t="s">
@@ -4485,7 +4484,7 @@
       <c r="AW13" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="AX13" s="20" t="s">
+      <c r="AX13" s="26" t="s">
         <v>58</v>
       </c>
       <c r="AY13" s="20" t="s">
@@ -4506,174 +4505,174 @@
       <c r="BD13" s="20"/>
       <c r="BE13" s="20"/>
     </row>
-    <row r="14" spans="1:57" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="31">
+    <row r="14" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14">
         <v>1927</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" t="s">
         <v>99</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14">
         <v>87</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14">
         <v>56</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14">
         <v>10.7</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="K14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="L14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="M14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="N14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="O14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="P14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q14" s="31">
+      <c r="I14" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14" t="s">
+        <v>58</v>
+      </c>
+      <c r="N14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" t="s">
+        <v>58</v>
+      </c>
+      <c r="P14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q14">
         <v>71</v>
       </c>
-      <c r="R14" s="31">
+      <c r="R14">
         <v>675</v>
       </c>
-      <c r="S14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="T14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="U14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="V14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="W14" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="X14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z14" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE14" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF14" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AK14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AM14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AO14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AP14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AQ14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AR14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AS14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AW14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AY14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="AZ14" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA14" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="BB14" s="31" t="s">
+      <c r="S14" t="s">
+        <v>58</v>
+      </c>
+      <c r="T14" t="s">
+        <v>58</v>
+      </c>
+      <c r="U14" t="s">
+        <v>58</v>
+      </c>
+      <c r="V14" t="s">
+        <v>58</v>
+      </c>
+      <c r="W14" t="b">
+        <v>0</v>
+      </c>
+      <c r="X14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU14" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX14" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>58</v>
+      </c>
+      <c r="BA14" t="b">
+        <v>0</v>
+      </c>
+      <c r="BB14" t="s">
         <v>70</v>
       </c>
-      <c r="BC14" s="31">
+      <c r="BC14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A15" t="b">
         <v>1</v>
       </c>
@@ -4812,7 +4811,7 @@
       <c r="AT15" t="s">
         <v>58</v>
       </c>
-      <c r="AU15" t="s">
+      <c r="AU15" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AV15" t="s">
@@ -4821,7 +4820,7 @@
       <c r="AW15" t="s">
         <v>58</v>
       </c>
-      <c r="AX15" t="s">
+      <c r="AX15" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AY15" t="s">
@@ -4840,7 +4839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A16" t="b">
         <v>1</v>
       </c>
@@ -4979,7 +4978,7 @@
       <c r="AT16" t="s">
         <v>58</v>
       </c>
-      <c r="AU16" t="s">
+      <c r="AU16" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AV16" t="s">
@@ -4988,7 +4987,7 @@
       <c r="AW16" t="s">
         <v>58</v>
       </c>
-      <c r="AX16" t="s">
+      <c r="AX16" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AY16" t="s">
@@ -5007,7 +5006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A17" t="b">
         <v>1</v>
       </c>
@@ -5146,7 +5145,7 @@
       <c r="AT17" t="s">
         <v>58</v>
       </c>
-      <c r="AU17" t="s">
+      <c r="AU17" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AV17" t="s">
@@ -5155,7 +5154,7 @@
       <c r="AW17" t="s">
         <v>58</v>
       </c>
-      <c r="AX17" t="s">
+      <c r="AX17" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AY17" t="s">
@@ -5174,7 +5173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A18" t="b">
         <v>1</v>
       </c>
@@ -5313,8 +5312,8 @@
       <c r="AT18" t="s">
         <v>58</v>
       </c>
-      <c r="AU18" s="2">
-        <v>37681</v>
+      <c r="AU18" s="25" t="s">
+        <v>565</v>
       </c>
       <c r="AV18">
         <v>2011</v>
@@ -5322,8 +5321,8 @@
       <c r="AW18" t="s">
         <v>58</v>
       </c>
-      <c r="AX18" s="2">
-        <v>39264</v>
+      <c r="AX18" s="25" t="s">
+        <v>567</v>
       </c>
       <c r="AY18">
         <v>2011</v>
@@ -5341,7 +5340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A19" t="b">
         <v>1</v>
       </c>
@@ -5480,8 +5479,8 @@
       <c r="AT19">
         <v>3</v>
       </c>
-      <c r="AU19" s="2">
-        <v>40057</v>
+      <c r="AU19" s="25" t="s">
+        <v>566</v>
       </c>
       <c r="AV19">
         <v>2012</v>
@@ -5489,8 +5488,8 @@
       <c r="AW19">
         <v>13</v>
       </c>
-      <c r="AX19" s="2">
-        <v>40848</v>
+      <c r="AX19" s="25" t="s">
+        <v>564</v>
       </c>
       <c r="AY19">
         <v>2012</v>
@@ -5508,7 +5507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
       <c r="A20" t="b">
         <v>1</v>
       </c>
@@ -5647,7 +5646,7 @@
       <c r="AT20" t="s">
         <v>58</v>
       </c>
-      <c r="AU20" t="s">
+      <c r="AU20" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AV20" t="s">
@@ -5656,7 +5655,7 @@
       <c r="AW20" t="s">
         <v>58</v>
       </c>
-      <c r="AX20" t="s">
+      <c r="AX20" s="25" t="s">
         <v>58</v>
       </c>
       <c r="AY20" t="s">
@@ -5675,14 +5674,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:55" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="b">
+    <row r="21" spans="1:55" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="b">
         <v>1</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21">
         <v>1693</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" t="s">
         <v>85</v>
       </c>
       <c r="D21" s="23">
@@ -5691,19 +5690,19 @@
       <c r="E21" s="23">
         <v>9</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="F21" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="H21" s="25" t="s">
+      <c r="H21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="K21" s="25" t="s">
+      <c r="K21" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="M21" s="25" t="s">
+      <c r="M21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="P21" s="25" t="s">
+      <c r="P21" s="24" t="s">
         <v>561</v>
       </c>
       <c r="Q21" s="23">
@@ -5712,19 +5711,19 @@
       <c r="R21" s="23">
         <v>331</v>
       </c>
-      <c r="S21" s="25" t="s">
+      <c r="S21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="T21" s="25" t="s">
+      <c r="T21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="V21" s="25" t="s">
+      <c r="V21" s="24" t="s">
         <v>561</v>
       </c>
       <c r="W21" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="Y21" s="25" t="s">
+      <c r="Y21" s="24" t="s">
         <v>561</v>
       </c>
       <c r="Z21" s="23" t="b">
@@ -5733,13 +5732,13 @@
       <c r="AA21" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="AB21" s="25" t="s">
+      <c r="AB21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="AC21" s="25" t="s">
+      <c r="AC21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="AD21" s="25" t="s">
+      <c r="AD21" s="24" t="s">
         <v>561</v>
       </c>
       <c r="AE21" s="23" t="b">
@@ -5748,61 +5747,102 @@
       <c r="AF21" s="23" t="b">
         <v>0</v>
       </c>
-      <c r="AG21" s="25" t="s">
+      <c r="AG21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="AH21" s="25" t="s">
+      <c r="AH21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="AI21" s="25" t="s">
+      <c r="AI21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="AJ21" s="25" t="s">
+      <c r="AJ21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="AK21" s="25" t="s">
+      <c r="AK21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="AL21" s="25" t="s">
+      <c r="AL21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="AM21" s="25" t="s">
+      <c r="AM21" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="AN21" s="25"/>
-      <c r="AR21" s="25" t="s">
+      <c r="AN21" s="24"/>
+      <c r="AR21" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="AS21" s="25" t="s">
+      <c r="AS21" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="AT21" s="25" t="s">
+      <c r="AT21" s="24" t="s">
         <v>561</v>
       </c>
       <c r="AU21" s="25" t="s">
+        <v>565</v>
+      </c>
+      <c r="AV21" s="24" t="s">
         <v>562</v>
       </c>
-      <c r="AV21" s="25" t="s">
-        <v>563</v>
-      </c>
-      <c r="AW21" s="25" t="s">
+      <c r="AW21" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="AX21" s="26" t="s">
-        <v>564</v>
-      </c>
-      <c r="AY21" s="25" t="s">
-        <v>563</v>
-      </c>
-      <c r="AZ21" s="25" t="s">
+      <c r="AX21" s="25" t="s">
+        <v>568</v>
+      </c>
+      <c r="AY21" s="24" t="s">
+        <v>562</v>
+      </c>
+      <c r="AZ21" s="24" t="s">
         <v>561</v>
       </c>
       <c r="BA21" s="23" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="24" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="AU24" s="2"/>
+      <c r="AX24" s="2"/>
+    </row>
+    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="AU29" s="20"/>
+      <c r="AX29" s="20"/>
+    </row>
+    <row r="30" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="AU30" s="20"/>
+      <c r="AX30" s="20"/>
+    </row>
+    <row r="31" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="AU31" s="20"/>
+      <c r="AX31" s="20"/>
+    </row>
+    <row r="32" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="AU32" s="20"/>
+      <c r="AX32" s="20"/>
+    </row>
+    <row r="33" spans="47:50" x14ac:dyDescent="0.3">
+      <c r="AU33" s="20"/>
+      <c r="AX33" s="20"/>
+    </row>
+    <row r="34" spans="47:50" x14ac:dyDescent="0.3">
+      <c r="AU34" s="20"/>
+      <c r="AX34" s="20"/>
+    </row>
+    <row r="39" spans="47:50" x14ac:dyDescent="0.3">
+      <c r="AU39" s="2"/>
+      <c r="AX39" s="2"/>
+    </row>
+    <row r="40" spans="47:50" x14ac:dyDescent="0.3">
+      <c r="AU40" s="2"/>
+      <c r="AX40" s="2"/>
+    </row>
+    <row r="42" spans="47:50" x14ac:dyDescent="0.3">
+      <c r="AU42" s="2"/>
+      <c r="AX42" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5814,12 +5854,12 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5890,7 +5930,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -5961,7 +6001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -6032,7 +6072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -6103,7 +6143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="b">
         <v>1</v>
       </c>
@@ -6119,48 +6159,44 @@
       <c r="E5" s="23">
         <v>62</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="24">
         <v>2004</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="24">
         <v>2005</v>
       </c>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="27" t="s">
+      <c r="N5" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="O5" s="27" t="s">
+      <c r="O5" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="P5" s="29">
+      <c r="P5" s="23">
         <v>252</v>
       </c>
-      <c r="Q5" s="27" t="s">
+      <c r="Q5" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="R5" s="28"/>
-      <c r="S5" s="27" t="s">
+      <c r="S5" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="T5" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="U5" s="28"/>
-      <c r="V5" s="29">
+      <c r="T5" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="V5" s="23">
         <v>227</v>
       </c>
       <c r="W5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -6176,41 +6212,37 @@
       <c r="E6" s="23">
         <v>31</v>
       </c>
-      <c r="H6" s="30">
+      <c r="H6" s="24">
         <v>1998</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="K6" s="30">
+      <c r="K6" s="24">
         <v>2000</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="27" t="s">
+      <c r="N6" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="O6" s="27" t="s">
+      <c r="O6" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="P6" s="29">
+      <c r="P6" s="23">
         <v>154</v>
       </c>
-      <c r="Q6" s="27" t="s">
+      <c r="Q6" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="R6" s="28"/>
-      <c r="S6" s="27" t="s">
+      <c r="S6" s="24" t="s">
         <v>561</v>
       </c>
-      <c r="T6" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="U6" s="28"/>
-      <c r="V6" s="29">
+      <c r="T6" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="V6" s="23">
         <v>128</v>
       </c>
       <c r="W6">
@@ -6230,14 +6262,14 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="132.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="108.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="49.7109375" customWidth="1"/>
+    <col min="4" max="4" width="132.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="108.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="49.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>144</v>
       </c>
@@ -6293,7 +6325,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>162</v>
       </c>
@@ -6340,7 +6372,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>162</v>
       </c>
@@ -6387,7 +6419,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>180</v>
       </c>
@@ -6434,7 +6466,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>180</v>
       </c>
@@ -6487,7 +6519,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>200</v>
       </c>
@@ -6534,7 +6566,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>200</v>
       </c>
@@ -6587,7 +6619,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>219</v>
       </c>
@@ -6631,7 +6663,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>219</v>
       </c>
@@ -6681,7 +6713,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
         <v>99</v>
       </c>
@@ -6728,7 +6760,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
         <v>99</v>
       </c>
@@ -6778,7 +6810,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
         <v>100</v>
       </c>
@@ -6831,7 +6863,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>100</v>
       </c>
@@ -6881,7 +6913,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>274</v>
       </c>
@@ -6934,7 +6966,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>274</v>
       </c>
@@ -6981,7 +7013,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>162</v>
       </c>
@@ -7028,7 +7060,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>162</v>
       </c>
@@ -7075,7 +7107,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>162</v>
       </c>
@@ -7119,7 +7151,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>200</v>
       </c>
@@ -7166,7 +7198,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>162</v>
       </c>
@@ -7219,7 +7251,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -7266,7 +7298,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>171</v>
       </c>
@@ -7313,7 +7345,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>171</v>
       </c>
@@ -7360,7 +7392,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>113</v>
       </c>
@@ -7407,7 +7439,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>180</v>
       </c>
@@ -7460,7 +7492,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>180</v>
       </c>
@@ -7510,7 +7542,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>180</v>
       </c>
@@ -7560,7 +7592,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>189</v>
       </c>
@@ -7610,7 +7642,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>189</v>
       </c>
@@ -7660,7 +7692,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>189</v>
       </c>
@@ -7707,7 +7739,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>200</v>
       </c>
@@ -7757,7 +7789,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>200</v>
       </c>
@@ -7807,7 +7839,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>200</v>
       </c>
@@ -7860,7 +7892,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="34" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
         <v>265</v>
       </c>
@@ -7913,7 +7945,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>274</v>
       </c>
@@ -7960,7 +7992,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>162</v>
       </c>
@@ -8007,7 +8039,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>219</v>
       </c>
@@ -8060,7 +8092,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>219</v>
       </c>
@@ -8113,7 +8145,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>219</v>
       </c>
@@ -8160,7 +8192,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="18" t="s">
         <v>99</v>
       </c>
@@ -8210,7 +8242,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
         <v>99</v>
       </c>
@@ -8260,7 +8292,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>162</v>
       </c>
@@ -8313,7 +8345,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>100</v>
       </c>
@@ -8366,7 +8398,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>100</v>
       </c>
@@ -8419,7 +8451,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="19" t="s">
         <v>100</v>
       </c>
@@ -8469,7 +8501,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>265</v>
       </c>
@@ -8519,7 +8551,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>265</v>
       </c>
@@ -8569,7 +8601,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="19" t="s">
         <v>274</v>
       </c>
@@ -8619,7 +8651,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
         <v>274</v>
       </c>

</xml_diff>